<commit_message>
He añadido el id del experimento y estoy con los evnetos de MOVE
</commit_message>
<xml_diff>
--- a/data_analysis/db_env/app/results/resultsALL.xlsx
+++ b/data_analysis/db_env/app/results/resultsALL.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:BW3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,37 +441,367 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>EXP_ID</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>GROUP</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>HMD</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>SCENARIO</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>TD</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>GP_N</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>GP_T</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>GP_T_SC</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>EXP_ID</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_R</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_L</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_1</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_1_R</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_1_L</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_2</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_2_R</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_2_L</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_3</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_3_R</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_3_L</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_4</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_4_R</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_4_L</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_a_2</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_a_3</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_a_4</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_a_5</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_a_7</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_a_9</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_R</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_L</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_SS</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_SS_R</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_SS_L</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_GR</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_GR_R</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_GR_L</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_SS_a_2</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_SS_a_3</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_SS_a_4</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_SS_a_5</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_SS_a_7</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_SS_a_9</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_GR_a_2</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_GR_a_3</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_GR_a_4</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_GR_a_5</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_GR_a_7</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_GR_a_9</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>EXP_ID</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_type_0</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_type_1</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_type_2</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_actor_1</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_actor_2</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_actor_3</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_actor_4</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_actor_5</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_actor_6</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_T</t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_T_SS</t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_T_C</t>
+        </is>
+      </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>EXP_ID</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>MV_N_VR</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>MV_N_RL</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>MV_D_VR</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>MV_D_RL</t>
+        </is>
+      </c>
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>MV_T_VR</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>MV_T_RL</t>
+        </is>
+      </c>
+      <c r="BW1" s="1" t="inlineStr">
+        <is>
+          <t>MV_T_TE</t>
         </is>
       </c>
     </row>
@@ -484,32 +814,230 @@
           <t>AA</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>TSV</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>QUEST</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>ALL</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>1433.02</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>24</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>57.914</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>52.486875</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>149</v>
+      </c>
+      <c r="M2" t="n">
+        <v>55</v>
+      </c>
+      <c r="N2" t="n">
+        <v>94</v>
+      </c>
+      <c r="O2" t="n">
+        <v>49</v>
+      </c>
+      <c r="P2" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>31</v>
+      </c>
+      <c r="R2" t="n">
+        <v>49</v>
+      </c>
+      <c r="S2" t="n">
+        <v>18</v>
+      </c>
+      <c r="T2" t="n">
+        <v>31</v>
+      </c>
+      <c r="U2" t="n">
+        <v>26</v>
+      </c>
+      <c r="V2" t="n">
+        <v>10</v>
+      </c>
+      <c r="W2" t="n">
+        <v>16</v>
+      </c>
+      <c r="X2" t="n">
+        <v>25</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>9</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>42</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>36</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>24</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>33</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>6</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>6</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>8.734</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>18.014</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>13.9</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.2462777777777778</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.332741935483871</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>19.885</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>15.22333333333333</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>24.547625</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.213</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.278</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0.363</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0.264</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>0.225</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>5.343</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>16.415</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>60.143</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>47.91</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>0.9360000000000001</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>0.858</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>14</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>7</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>7</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>2</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>6</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>2</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>4</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>76.73999999999999</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>22.7205</v>
+      </c>
+      <c r="BO2" t="n">
+        <v>44.81325</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>200</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>351</v>
+      </c>
+      <c r="BS2" t="n">
+        <v>635.75</v>
+      </c>
+      <c r="BT2" t="n">
+        <v>104.02</v>
+      </c>
+      <c r="BU2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BV2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BW2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -521,32 +1049,230 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>CTRL</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>QUEST</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>ALL</t>
         </is>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>1236.99</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>24</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>49.323</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>43.423375</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" t="n">
+        <v>146</v>
+      </c>
+      <c r="M3" t="n">
+        <v>112</v>
+      </c>
+      <c r="N3" t="n">
+        <v>34</v>
+      </c>
+      <c r="O3" t="n">
+        <v>43</v>
+      </c>
+      <c r="P3" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>11</v>
+      </c>
+      <c r="R3" t="n">
+        <v>43</v>
+      </c>
+      <c r="S3" t="n">
+        <v>32</v>
+      </c>
+      <c r="T3" t="n">
+        <v>11</v>
+      </c>
+      <c r="U3" t="n">
+        <v>30</v>
+      </c>
+      <c r="V3" t="n">
+        <v>24</v>
+      </c>
+      <c r="W3" t="n">
+        <v>6</v>
+      </c>
+      <c r="X3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>24</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>42</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>36</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>14</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>7.745</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>10.082</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>34.031</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0.367</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>0.22934375</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>0.505</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>33.431</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>12.91883333333333</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>53.943</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>0.454</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0.237</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>0.266</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>0.139</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>0.119</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>3.752</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>8.432</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>157.554</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>27.393</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>12</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>6</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>6</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>2</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>4</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>2</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>4</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>78.679</v>
+      </c>
+      <c r="BN3" t="n">
+        <v>22.591</v>
+      </c>
+      <c r="BO3" t="n">
+        <v>53.86566666666666</v>
+      </c>
+      <c r="BP3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ3" t="n">
+        <v>237</v>
+      </c>
+      <c r="BR3" t="n">
+        <v>442</v>
+      </c>
+      <c r="BS3" t="n">
+        <v>666.009</v>
+      </c>
+      <c r="BT3" t="n">
+        <v>118.252</v>
+      </c>
+      <c r="BU3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BV3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BW3" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Estaba con la analisis de los formularios
</commit_message>
<xml_diff>
--- a/data_analysis/db_env/app/results/resultsALL.xlsx
+++ b/data_analysis/db_env/app/results/resultsALL.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:CW3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,57 +461,477 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>TD</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>GP_N</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>GP_T</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>EXP_ID</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_R</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_L</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_1</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_1_R</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_1_L</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_2</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_2_R</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_2_L</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_3</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_3_R</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_3_L</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_4</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_4_R</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_t_4_L</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_a_2</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_a_3</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_a_4</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_a_5</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_a_7</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>OI_N_a_9</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_R</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_L</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_SS</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_SS_R</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_SS_L</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_GR</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_GR_R</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_GR_L</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_SS_a_2</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_SS_a_3</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_SS_a_4</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_SS_a_5</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_SS_a_7</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_SS_a_9</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_GR_a_2</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_GR_a_3</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_GR_a_4</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_GR_a_5</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_GR_a_7</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>OI_T_GR_a_9</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>EXP_ID</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_type_0</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_type_1</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_type_2</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_actor_1</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_actor_2</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_actor_3</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_actor_4</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_actor_5</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_actor_6</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_T</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_T_SS</t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_T_C</t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
+          <t>EXP_ID</t>
+        </is>
+      </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>MV_N_VR</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>MV_N_RL</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>MV_DT_VR</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>MV_DT_RL</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>MV_DM_VR</t>
+        </is>
+      </c>
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>MV_DM_RL</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>MV_T_VR</t>
+        </is>
+      </c>
+      <c r="BW1" s="1" t="inlineStr">
+        <is>
+          <t>MV_T_RL</t>
+        </is>
+      </c>
+      <c r="BX1" s="1" t="inlineStr">
+        <is>
+          <t>MV_T_TE</t>
+        </is>
+      </c>
+      <c r="BY1" s="1" t="inlineStr">
+        <is>
+          <t>EXP_ID</t>
+        </is>
+      </c>
+      <c r="BZ1" s="1" t="inlineStr">
+        <is>
           <t>UI_N</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N_t_0</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="CA1" s="1" t="inlineStr">
+        <is>
+          <t>UI_N_R</t>
+        </is>
+      </c>
+      <c r="CB1" s="1" t="inlineStr">
+        <is>
+          <t>UI_N_L</t>
+        </is>
+      </c>
+      <c r="CC1" s="1" t="inlineStr">
         <is>
           <t>UI_N_t_1</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="CD1" s="1" t="inlineStr">
+        <is>
+          <t>UI_N_t_1_R</t>
+        </is>
+      </c>
+      <c r="CE1" s="1" t="inlineStr">
+        <is>
+          <t>UI_N_t_1_L</t>
+        </is>
+      </c>
+      <c r="CF1" s="1" t="inlineStr">
         <is>
           <t>UI_N_t_2</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="CG1" s="1" t="inlineStr">
+        <is>
+          <t>UI_N_t_2_R</t>
+        </is>
+      </c>
+      <c r="CH1" s="1" t="inlineStr">
+        <is>
+          <t>UI_N_t_2_L</t>
+        </is>
+      </c>
+      <c r="CI1" s="1" t="inlineStr">
         <is>
           <t>UI_N_t_3</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="CJ1" s="1" t="inlineStr">
+        <is>
+          <t>UI_N_t_3_R</t>
+        </is>
+      </c>
+      <c r="CK1" s="1" t="inlineStr">
+        <is>
+          <t>UI_N_t_3_L</t>
+        </is>
+      </c>
+      <c r="CL1" s="1" t="inlineStr">
         <is>
           <t>UI_N_t_4</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N_t_5</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N_t_6</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N_t_7</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N_t_8</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="CM1" s="1" t="inlineStr">
+        <is>
+          <t>UI_N_t_4_R</t>
+        </is>
+      </c>
+      <c r="CN1" s="1" t="inlineStr">
+        <is>
+          <t>UI_N_t_4_L</t>
+        </is>
+      </c>
+      <c r="CO1" s="1" t="inlineStr">
         <is>
           <t>UI_T</t>
+        </is>
+      </c>
+      <c r="CP1" s="1" t="inlineStr">
+        <is>
+          <t>UI_T_SC</t>
+        </is>
+      </c>
+      <c r="CQ1" s="1" t="inlineStr">
+        <is>
+          <t>UI_T_SC_t_1</t>
+        </is>
+      </c>
+      <c r="CR1" s="1" t="inlineStr">
+        <is>
+          <t>UI_T_SC_t_2</t>
+        </is>
+      </c>
+      <c r="CS1" s="1" t="inlineStr">
+        <is>
+          <t>UI_T_SC_t_3</t>
+        </is>
+      </c>
+      <c r="CT1" s="1" t="inlineStr">
+        <is>
+          <t>UI_T_SC_t_4</t>
+        </is>
+      </c>
+      <c r="CU1" s="1" t="inlineStr">
+        <is>
+          <t>EXP_ID</t>
+        </is>
+      </c>
+      <c r="CV1" s="1" t="inlineStr">
+        <is>
+          <t>TT_T</t>
+        </is>
+      </c>
+      <c r="CW1" s="1" t="inlineStr">
+        <is>
+          <t>EXP_ID</t>
         </is>
       </c>
     </row>
@@ -543,37 +963,289 @@
         </is>
       </c>
       <c r="G2" t="n">
+        <v>1433.02</v>
+      </c>
+      <c r="H2" t="n">
+        <v>24</v>
+      </c>
+      <c r="I2" t="n">
+        <v>52.486875</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>149</v>
+      </c>
+      <c r="L2" t="n">
+        <v>55</v>
+      </c>
+      <c r="M2" t="n">
+        <v>94</v>
+      </c>
+      <c r="N2" t="n">
+        <v>49</v>
+      </c>
+      <c r="O2" t="n">
+        <v>18</v>
+      </c>
+      <c r="P2" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>49</v>
+      </c>
+      <c r="R2" t="n">
+        <v>18</v>
+      </c>
+      <c r="S2" t="n">
+        <v>31</v>
+      </c>
+      <c r="T2" t="n">
+        <v>26</v>
+      </c>
+      <c r="U2" t="n">
+        <v>10</v>
+      </c>
+      <c r="V2" t="n">
+        <v>16</v>
+      </c>
+      <c r="W2" t="n">
+        <v>25</v>
+      </c>
+      <c r="X2" t="n">
+        <v>9</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>16</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>42</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>36</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>33</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>6</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>8.734</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>18.014</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>13.9</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.2462777777777778</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.332741935483871</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>19.885</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>15.22333333333333</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>24.547625</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.213</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.278</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.363</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0.451</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>5.343</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>16.415</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>60.143</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>47.91</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>1.872</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>1.716</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>14</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>7</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>7</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>2</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>6</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>2</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>4</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>76.73999999999999</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>20.78028571428571</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>44.81325</v>
+      </c>
+      <c r="BO2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>198</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>345</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>583.15</v>
+      </c>
+      <c r="BS2" t="n">
+        <v>56.195</v>
+      </c>
+      <c r="BT2" t="n">
+        <v>2.945</v>
+      </c>
+      <c r="BU2" t="n">
+        <v>0.163</v>
+      </c>
+      <c r="BV2" t="n">
+        <v>6.142</v>
+      </c>
+      <c r="BW2" t="n">
+        <v>0.314</v>
+      </c>
+      <c r="BX2" t="n">
+        <v>0.644</v>
+      </c>
+      <c r="BY2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BZ2" t="n">
         <v>818</v>
       </c>
-      <c r="H2" t="n">
+      <c r="CA2" t="n">
+        <v>670</v>
+      </c>
+      <c r="CB2" t="n">
+        <v>148</v>
+      </c>
+      <c r="CC2" t="n">
+        <v>418</v>
+      </c>
+      <c r="CD2" t="n">
+        <v>392</v>
+      </c>
+      <c r="CE2" t="n">
+        <v>26</v>
+      </c>
+      <c r="CF2" t="n">
+        <v>268</v>
+      </c>
+      <c r="CG2" t="n">
+        <v>210</v>
+      </c>
+      <c r="CH2" t="n">
+        <v>58</v>
+      </c>
+      <c r="CI2" t="n">
+        <v>116</v>
+      </c>
+      <c r="CJ2" t="n">
+        <v>52</v>
+      </c>
+      <c r="CK2" t="n">
+        <v>64</v>
+      </c>
+      <c r="CL2" t="n">
+        <v>16</v>
+      </c>
+      <c r="CM2" t="n">
+        <v>16</v>
+      </c>
+      <c r="CN2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="n">
-        <v>26</v>
-      </c>
-      <c r="J2" t="n">
-        <v>392</v>
-      </c>
-      <c r="K2" t="n">
-        <v>58</v>
-      </c>
-      <c r="L2" t="n">
-        <v>210</v>
-      </c>
-      <c r="M2" t="n">
-        <v>64</v>
-      </c>
-      <c r="N2" t="n">
-        <v>52</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>16</v>
-      </c>
-      <c r="Q2" t="n">
+      <c r="CO2" t="n">
         <v>1.73</v>
+      </c>
+      <c r="CP2" t="n">
+        <v>3.202</v>
+      </c>
+      <c r="CQ2" t="n">
+        <v>0.542</v>
+      </c>
+      <c r="CR2" t="n">
+        <v>0.173</v>
+      </c>
+      <c r="CS2" t="n">
+        <v>9.207000000000001</v>
+      </c>
+      <c r="CT2" t="n">
+        <v>0.203</v>
+      </c>
+      <c r="CU2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CV2" t="n">
+        <v>19.0045</v>
+      </c>
+      <c r="CW2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -604,39 +1276,293 @@
         </is>
       </c>
       <c r="G3" t="n">
+        <v>1236.99</v>
+      </c>
+      <c r="H3" t="n">
+        <v>24</v>
+      </c>
+      <c r="I3" t="n">
+        <v>43.423375</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
+        <v>146</v>
+      </c>
+      <c r="L3" t="n">
+        <v>112</v>
+      </c>
+      <c r="M3" t="n">
+        <v>34</v>
+      </c>
+      <c r="N3" t="n">
+        <v>43</v>
+      </c>
+      <c r="O3" t="n">
+        <v>32</v>
+      </c>
+      <c r="P3" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>43</v>
+      </c>
+      <c r="R3" t="n">
+        <v>32</v>
+      </c>
+      <c r="S3" t="n">
+        <v>11</v>
+      </c>
+      <c r="T3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U3" t="n">
+        <v>24</v>
+      </c>
+      <c r="V3" t="n">
+        <v>6</v>
+      </c>
+      <c r="W3" t="n">
+        <v>30</v>
+      </c>
+      <c r="X3" t="n">
+        <v>24</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>42</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>36</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>14</v>
+      </c>
+      <c r="AD3" t="n">
         <v>0</v>
       </c>
-      <c r="H3" t="n">
+      <c r="AE3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>7.745</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>10.082</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>34.031</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0.367</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0.22934375</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>0.505</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>33.431</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>12.91883333333333</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>53.943</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>0.454</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>0.237</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0.266</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>0.279</v>
+      </c>
+      <c r="AS3" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="AT3" t="n">
+        <v>0.237</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>3.752</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>8.432</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>157.554</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>54.786</v>
+      </c>
+      <c r="AY3" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="AZ3" t="n">
+        <v>0.961</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>12</v>
+      </c>
+      <c r="BC3" t="n">
         <v>0</v>
       </c>
-      <c r="I3" t="n">
+      <c r="BD3" t="n">
+        <v>6</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>6</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>2</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>4</v>
+      </c>
+      <c r="BH3" t="n">
         <v>0</v>
       </c>
-      <c r="J3" t="n">
+      <c r="BI3" t="n">
         <v>0</v>
       </c>
-      <c r="K3" t="n">
+      <c r="BJ3" t="n">
+        <v>2</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>4</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>78.679</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>23.34616666666667</v>
+      </c>
+      <c r="BN3" t="n">
+        <v>53.86566666666666</v>
+      </c>
+      <c r="BO3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP3" t="n">
+        <v>235</v>
+      </c>
+      <c r="BQ3" t="n">
+        <v>437</v>
+      </c>
+      <c r="BR3" t="n">
+        <v>615.752</v>
+      </c>
+      <c r="BS3" t="n">
+        <v>75.69499999999999</v>
+      </c>
+      <c r="BT3" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="BU3" t="n">
+        <v>0.173</v>
+      </c>
+      <c r="BV3" t="n">
+        <v>4.653</v>
+      </c>
+      <c r="BW3" t="n">
+        <v>0.112</v>
+      </c>
+      <c r="BX3" t="n">
+        <v>0.312</v>
+      </c>
+      <c r="BY3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BZ3" t="n">
+        <v>760</v>
+      </c>
+      <c r="CA3" t="n">
+        <v>696</v>
+      </c>
+      <c r="CB3" t="n">
+        <v>64</v>
+      </c>
+      <c r="CC3" t="n">
+        <v>508</v>
+      </c>
+      <c r="CD3" t="n">
+        <v>484</v>
+      </c>
+      <c r="CE3" t="n">
+        <v>24</v>
+      </c>
+      <c r="CF3" t="n">
+        <v>170</v>
+      </c>
+      <c r="CG3" t="n">
+        <v>148</v>
+      </c>
+      <c r="CH3" t="n">
+        <v>22</v>
+      </c>
+      <c r="CI3" t="n">
+        <v>76</v>
+      </c>
+      <c r="CJ3" t="n">
+        <v>58</v>
+      </c>
+      <c r="CK3" t="n">
+        <v>18</v>
+      </c>
+      <c r="CL3" t="n">
+        <v>6</v>
+      </c>
+      <c r="CM3" t="n">
+        <v>6</v>
+      </c>
+      <c r="CN3" t="n">
         <v>0</v>
       </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
+      <c r="CO3" t="n">
+        <v>1.595</v>
+      </c>
+      <c r="CP3" t="n">
+        <v>5.745</v>
+      </c>
+      <c r="CQ3" t="n">
+        <v>0.413</v>
+      </c>
+      <c r="CR3" t="n">
+        <v>0.113</v>
+      </c>
+      <c r="CS3" t="n">
+        <v>23.445</v>
+      </c>
+      <c r="CT3" t="n">
+        <v>0.103</v>
+      </c>
+      <c r="CU3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CV3" t="n">
+        <v>16.3112</v>
+      </c>
+      <c r="CW3" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se añaden los resultados del FORM a los resultados finales. Hay que revisar que son correctos.
</commit_message>
<xml_diff>
--- a/data_analysis/db_env/app/results/resultsALL.xlsx
+++ b/data_analysis/db_env/app/results/resultsALL.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CW3"/>
+  <dimension ref="A1:BU3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -691,247 +691,107 @@
       </c>
       <c r="BA1" s="1" t="inlineStr">
         <is>
-          <t>EXP_ID</t>
+          <t>APP</t>
         </is>
       </c>
       <c r="BB1" s="1" t="inlineStr">
         <is>
-          <t>NPC_N</t>
+          <t>UX_A</t>
         </is>
       </c>
       <c r="BC1" s="1" t="inlineStr">
         <is>
-          <t>NPC_N_type_0</t>
+          <t>UX_P</t>
         </is>
       </c>
       <c r="BD1" s="1" t="inlineStr">
         <is>
-          <t>NPC_N_type_1</t>
+          <t>UX_E</t>
         </is>
       </c>
       <c r="BE1" s="1" t="inlineStr">
         <is>
-          <t>NPC_N_type_2</t>
+          <t>UX_D</t>
         </is>
       </c>
       <c r="BF1" s="1" t="inlineStr">
         <is>
-          <t>NPC_N_actor_1</t>
+          <t>UX_S</t>
         </is>
       </c>
       <c r="BG1" s="1" t="inlineStr">
         <is>
-          <t>NPC_N_actor_2</t>
+          <t>UX_N</t>
         </is>
       </c>
       <c r="BH1" s="1" t="inlineStr">
         <is>
-          <t>NPC_N_actor_3</t>
+          <t>SUS</t>
         </is>
       </c>
       <c r="BI1" s="1" t="inlineStr">
         <is>
-          <t>NPC_N_actor_4</t>
+          <t>CL_W_MD</t>
         </is>
       </c>
       <c r="BJ1" s="1" t="inlineStr">
         <is>
-          <t>NPC_N_actor_5</t>
+          <t>CL_W_PD</t>
         </is>
       </c>
       <c r="BK1" s="1" t="inlineStr">
         <is>
-          <t>NPC_N_actor_6</t>
+          <t>CL_W_TD</t>
         </is>
       </c>
       <c r="BL1" s="1" t="inlineStr">
         <is>
-          <t>NPC_T</t>
+          <t>CL_W_E</t>
         </is>
       </c>
       <c r="BM1" s="1" t="inlineStr">
         <is>
-          <t>NPC_T_SS</t>
+          <t>CL_W_P</t>
         </is>
       </c>
       <c r="BN1" s="1" t="inlineStr">
         <is>
-          <t>NPC_T_C</t>
+          <t>CL_W_F</t>
         </is>
       </c>
       <c r="BO1" s="1" t="inlineStr">
         <is>
-          <t>EXP_ID</t>
+          <t>CL_MD</t>
         </is>
       </c>
       <c r="BP1" s="1" t="inlineStr">
         <is>
-          <t>MV_N_VR</t>
+          <t>CL_PD</t>
         </is>
       </c>
       <c r="BQ1" s="1" t="inlineStr">
         <is>
-          <t>MV_N_RL</t>
+          <t>CL_TD</t>
         </is>
       </c>
       <c r="BR1" s="1" t="inlineStr">
         <is>
-          <t>MV_DT_VR</t>
+          <t>CL_E</t>
         </is>
       </c>
       <c r="BS1" s="1" t="inlineStr">
         <is>
-          <t>MV_DT_RL</t>
+          <t>CL_P</t>
         </is>
       </c>
       <c r="BT1" s="1" t="inlineStr">
         <is>
-          <t>MV_DM_VR</t>
+          <t>CL_F</t>
         </is>
       </c>
       <c r="BU1" s="1" t="inlineStr">
         <is>
-          <t>MV_DM_RL</t>
-        </is>
-      </c>
-      <c r="BV1" s="1" t="inlineStr">
-        <is>
-          <t>MV_T_VR</t>
-        </is>
-      </c>
-      <c r="BW1" s="1" t="inlineStr">
-        <is>
-          <t>MV_T_RL</t>
-        </is>
-      </c>
-      <c r="BX1" s="1" t="inlineStr">
-        <is>
-          <t>MV_T_TE</t>
-        </is>
-      </c>
-      <c r="BY1" s="1" t="inlineStr">
-        <is>
-          <t>EXP_ID</t>
-        </is>
-      </c>
-      <c r="BZ1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N</t>
-        </is>
-      </c>
-      <c r="CA1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N_R</t>
-        </is>
-      </c>
-      <c r="CB1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N_L</t>
-        </is>
-      </c>
-      <c r="CC1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N_t_1</t>
-        </is>
-      </c>
-      <c r="CD1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N_t_1_R</t>
-        </is>
-      </c>
-      <c r="CE1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N_t_1_L</t>
-        </is>
-      </c>
-      <c r="CF1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N_t_2</t>
-        </is>
-      </c>
-      <c r="CG1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N_t_2_R</t>
-        </is>
-      </c>
-      <c r="CH1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N_t_2_L</t>
-        </is>
-      </c>
-      <c r="CI1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N_t_3</t>
-        </is>
-      </c>
-      <c r="CJ1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N_t_3_R</t>
-        </is>
-      </c>
-      <c r="CK1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N_t_3_L</t>
-        </is>
-      </c>
-      <c r="CL1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N_t_4</t>
-        </is>
-      </c>
-      <c r="CM1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N_t_4_R</t>
-        </is>
-      </c>
-      <c r="CN1" s="1" t="inlineStr">
-        <is>
-          <t>UI_N_t_4_L</t>
-        </is>
-      </c>
-      <c r="CO1" s="1" t="inlineStr">
-        <is>
-          <t>UI_T</t>
-        </is>
-      </c>
-      <c r="CP1" s="1" t="inlineStr">
-        <is>
-          <t>UI_T_SC</t>
-        </is>
-      </c>
-      <c r="CQ1" s="1" t="inlineStr">
-        <is>
-          <t>UI_T_SC_t_1</t>
-        </is>
-      </c>
-      <c r="CR1" s="1" t="inlineStr">
-        <is>
-          <t>UI_T_SC_t_2</t>
-        </is>
-      </c>
-      <c r="CS1" s="1" t="inlineStr">
-        <is>
-          <t>UI_T_SC_t_3</t>
-        </is>
-      </c>
-      <c r="CT1" s="1" t="inlineStr">
-        <is>
-          <t>UI_T_SC_t_4</t>
-        </is>
-      </c>
-      <c r="CU1" s="1" t="inlineStr">
-        <is>
-          <t>EXP_ID</t>
-        </is>
-      </c>
-      <c r="CV1" s="1" t="inlineStr">
-        <is>
-          <t>TT_T</t>
-        </is>
-      </c>
-      <c r="CW1" s="1" t="inlineStr">
-        <is>
-          <t>EXP_ID</t>
+          <t>CL_SCORE</t>
         </is>
       </c>
     </row>
@@ -1101,151 +961,67 @@
         <v>1.716</v>
       </c>
       <c r="BA2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB2" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="BC2" t="n">
         <v>0</v>
       </c>
       <c r="BD2" t="n">
-        <v>7</v>
+        <v>0.25</v>
       </c>
       <c r="BE2" t="n">
-        <v>7</v>
+        <v>-0.75</v>
       </c>
       <c r="BF2" t="n">
-        <v>2</v>
+        <v>0.25</v>
       </c>
       <c r="BG2" t="n">
-        <v>6</v>
+        <v>1.5</v>
       </c>
       <c r="BH2" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="BI2" t="n">
-        <v>0</v>
+        <v>0.133</v>
       </c>
       <c r="BJ2" t="n">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="BK2" t="n">
-        <v>4</v>
+        <v>0.067</v>
       </c>
       <c r="BL2" t="n">
-        <v>76.73999999999999</v>
+        <v>0.2</v>
       </c>
       <c r="BM2" t="n">
-        <v>20.78028571428571</v>
+        <v>0.067</v>
       </c>
       <c r="BN2" t="n">
-        <v>44.81325</v>
+        <v>0.333</v>
       </c>
       <c r="BO2" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="BP2" t="n">
-        <v>198</v>
+        <v>1.4</v>
       </c>
       <c r="BQ2" t="n">
-        <v>345</v>
+        <v>0.133</v>
       </c>
       <c r="BR2" t="n">
-        <v>583.15</v>
+        <v>0.8</v>
       </c>
       <c r="BS2" t="n">
-        <v>56.195</v>
+        <v>0.6</v>
       </c>
       <c r="BT2" t="n">
-        <v>2.945</v>
+        <v>0.333</v>
       </c>
       <c r="BU2" t="n">
-        <v>0.163</v>
-      </c>
-      <c r="BV2" t="n">
-        <v>6.142</v>
-      </c>
-      <c r="BW2" t="n">
-        <v>0.314</v>
-      </c>
-      <c r="BX2" t="n">
-        <v>0.644</v>
-      </c>
-      <c r="BY2" t="n">
-        <v>1</v>
-      </c>
-      <c r="BZ2" t="n">
-        <v>818</v>
-      </c>
-      <c r="CA2" t="n">
-        <v>670</v>
-      </c>
-      <c r="CB2" t="n">
-        <v>148</v>
-      </c>
-      <c r="CC2" t="n">
-        <v>418</v>
-      </c>
-      <c r="CD2" t="n">
-        <v>392</v>
-      </c>
-      <c r="CE2" t="n">
-        <v>26</v>
-      </c>
-      <c r="CF2" t="n">
-        <v>268</v>
-      </c>
-      <c r="CG2" t="n">
-        <v>210</v>
-      </c>
-      <c r="CH2" t="n">
-        <v>58</v>
-      </c>
-      <c r="CI2" t="n">
-        <v>116</v>
-      </c>
-      <c r="CJ2" t="n">
-        <v>52</v>
-      </c>
-      <c r="CK2" t="n">
-        <v>64</v>
-      </c>
-      <c r="CL2" t="n">
-        <v>16</v>
-      </c>
-      <c r="CM2" t="n">
-        <v>16</v>
-      </c>
-      <c r="CN2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CO2" t="n">
-        <v>1.73</v>
-      </c>
-      <c r="CP2" t="n">
-        <v>3.202</v>
-      </c>
-      <c r="CQ2" t="n">
-        <v>0.542</v>
-      </c>
-      <c r="CR2" t="n">
-        <v>0.173</v>
-      </c>
-      <c r="CS2" t="n">
-        <v>9.207000000000001</v>
-      </c>
-      <c r="CT2" t="n">
-        <v>0.203</v>
-      </c>
-      <c r="CU2" t="n">
-        <v>1</v>
-      </c>
-      <c r="CV2" t="n">
-        <v>19.0045</v>
-      </c>
-      <c r="CW2" t="n">
-        <v>1</v>
+        <v>4.666</v>
       </c>
     </row>
     <row r="3">
@@ -1418,151 +1194,67 @@
         <v>0.961</v>
       </c>
       <c r="BA3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB3" t="n">
-        <v>12</v>
+        <v>-0.333</v>
       </c>
       <c r="BC3" t="n">
         <v>0</v>
       </c>
       <c r="BD3" t="n">
-        <v>6</v>
+        <v>0.25</v>
       </c>
       <c r="BE3" t="n">
-        <v>6</v>
+        <v>-0.25</v>
       </c>
       <c r="BF3" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="BG3" t="n">
-        <v>4</v>
+        <v>-0.25</v>
       </c>
       <c r="BH3" t="n">
+        <v>92.5</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>0.067</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>0.267</v>
+      </c>
+      <c r="BN3" t="n">
         <v>0</v>
       </c>
-      <c r="BI3" t="n">
+      <c r="BO3" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="BP3" t="n">
+        <v>0.067</v>
+      </c>
+      <c r="BQ3" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="BR3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="BS3" t="n">
+        <v>2.133</v>
+      </c>
+      <c r="BT3" t="n">
         <v>0</v>
       </c>
-      <c r="BJ3" t="n">
-        <v>2</v>
-      </c>
-      <c r="BK3" t="n">
-        <v>4</v>
-      </c>
-      <c r="BL3" t="n">
-        <v>78.679</v>
-      </c>
-      <c r="BM3" t="n">
-        <v>23.34616666666667</v>
-      </c>
-      <c r="BN3" t="n">
-        <v>53.86566666666666</v>
-      </c>
-      <c r="BO3" t="n">
-        <v>1</v>
-      </c>
-      <c r="BP3" t="n">
-        <v>235</v>
-      </c>
-      <c r="BQ3" t="n">
-        <v>437</v>
-      </c>
-      <c r="BR3" t="n">
-        <v>615.752</v>
-      </c>
-      <c r="BS3" t="n">
-        <v>75.69499999999999</v>
-      </c>
-      <c r="BT3" t="n">
-        <v>2.62</v>
-      </c>
       <c r="BU3" t="n">
-        <v>0.173</v>
-      </c>
-      <c r="BV3" t="n">
-        <v>4.653</v>
-      </c>
-      <c r="BW3" t="n">
-        <v>0.112</v>
-      </c>
-      <c r="BX3" t="n">
-        <v>0.312</v>
-      </c>
-      <c r="BY3" t="n">
-        <v>1</v>
-      </c>
-      <c r="BZ3" t="n">
-        <v>760</v>
-      </c>
-      <c r="CA3" t="n">
-        <v>696</v>
-      </c>
-      <c r="CB3" t="n">
-        <v>64</v>
-      </c>
-      <c r="CC3" t="n">
-        <v>508</v>
-      </c>
-      <c r="CD3" t="n">
-        <v>484</v>
-      </c>
-      <c r="CE3" t="n">
-        <v>24</v>
-      </c>
-      <c r="CF3" t="n">
-        <v>170</v>
-      </c>
-      <c r="CG3" t="n">
-        <v>148</v>
-      </c>
-      <c r="CH3" t="n">
-        <v>22</v>
-      </c>
-      <c r="CI3" t="n">
-        <v>76</v>
-      </c>
-      <c r="CJ3" t="n">
-        <v>58</v>
-      </c>
-      <c r="CK3" t="n">
-        <v>18</v>
-      </c>
-      <c r="CL3" t="n">
-        <v>6</v>
-      </c>
-      <c r="CM3" t="n">
-        <v>6</v>
-      </c>
-      <c r="CN3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CO3" t="n">
-        <v>1.595</v>
-      </c>
-      <c r="CP3" t="n">
-        <v>5.745</v>
-      </c>
-      <c r="CQ3" t="n">
-        <v>0.413</v>
-      </c>
-      <c r="CR3" t="n">
-        <v>0.113</v>
-      </c>
-      <c r="CS3" t="n">
-        <v>23.445</v>
-      </c>
-      <c r="CT3" t="n">
-        <v>0.103</v>
-      </c>
-      <c r="CU3" t="n">
-        <v>1</v>
-      </c>
-      <c r="CV3" t="n">
-        <v>16.3112</v>
-      </c>
-      <c r="CW3" t="n">
-        <v>1</v>
+        <v>4.066</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Estoy ordenando un poco el código del analisis. Es que al meter el analisis del formulario se ha quedado un poco raro y ya estaba con codigo espagueti. Y mi señor director de tesis quiere que la aplicación (sin tener ni idea de lo que pasará en los próximos 15 años) funcione para los próximos 15 años (más los que le salga de las narices ese día cuando se levante).
</commit_message>
<xml_diff>
--- a/data_analysis/db_env/app/results/resultsALL.xlsx
+++ b/data_analysis/db_env/app/results/resultsALL.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BU3"/>
+  <dimension ref="A1:AZ3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,357 +441,252 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>EXP_ID</t>
+          <t>SCENARIO</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>GROUP</t>
+          <t>TD</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>HMD</t>
+          <t>GP_N</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>SCENARIO</t>
+          <t>GP_T</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>TD</t>
+          <t>OI_N</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>GP_N</t>
+          <t>OI_N_R</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>GP_T</t>
+          <t>OI_N_L</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>EXP_ID</t>
+          <t>OI_N_t_1</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>OI_N</t>
+          <t>OI_N_t_1_R</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_R</t>
+          <t>OI_N_t_1_L</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_L</t>
+          <t>OI_N_t_2</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_1</t>
+          <t>OI_N_t_2_R</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_1_R</t>
+          <t>OI_N_t_2_L</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_1_L</t>
+          <t>OI_N_t_3</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_2</t>
+          <t>OI_N_t_3_R</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_2_R</t>
+          <t>OI_N_t_3_L</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_2_L</t>
+          <t>OI_N_t_4</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_3</t>
+          <t>OI_N_t_4_R</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_3_R</t>
+          <t>OI_N_t_4_L</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_3_L</t>
+          <t>OI_N_a_2</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_4</t>
+          <t>OI_N_a_3</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_4_R</t>
+          <t>OI_N_a_4</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_4_L</t>
+          <t>OI_N_a_5</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_a_2</t>
+          <t>OI_N_a_7</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_a_3</t>
+          <t>OI_N_a_9</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_a_4</t>
+          <t>OI_T</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_a_5</t>
+          <t>OI_T_R</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_a_7</t>
+          <t>OI_T_L</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_a_9</t>
+          <t>OI_T_SS</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>OI_T</t>
+          <t>OI_T_SS_R</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_R</t>
+          <t>OI_T_SS_L</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_L</t>
+          <t>OI_T_GR</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_SS</t>
+          <t>OI_T_GR_R</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_SS_R</t>
+          <t>OI_T_GR_L</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_SS_L</t>
+          <t>OI_T_SS_a_2</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_GR</t>
+          <t>OI_T_SS_a_3</t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_GR_R</t>
+          <t>OI_T_SS_a_4</t>
         </is>
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_GR_L</t>
+          <t>OI_T_SS_a_5</t>
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_SS_a_2</t>
+          <t>OI_T_SS_a_7</t>
         </is>
       </c>
       <c r="AP1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_SS_a_3</t>
+          <t>OI_T_SS_a_9</t>
         </is>
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_SS_a_4</t>
+          <t>OI_T_GR_a_2</t>
         </is>
       </c>
       <c r="AR1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_SS_a_5</t>
+          <t>OI_T_GR_a_3</t>
         </is>
       </c>
       <c r="AS1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_SS_a_7</t>
+          <t>OI_T_GR_a_4</t>
         </is>
       </c>
       <c r="AT1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_SS_a_9</t>
+          <t>OI_T_GR_a_5</t>
         </is>
       </c>
       <c r="AU1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_GR_a_2</t>
+          <t>OI_T_GR_a_7</t>
         </is>
       </c>
       <c r="AV1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_GR_a_3</t>
+          <t>OI_T_GR_a_9</t>
         </is>
       </c>
       <c r="AW1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_GR_a_4</t>
+          <t>AGE</t>
         </is>
       </c>
       <c r="AX1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_GR_a_5</t>
+          <t>GENRE</t>
         </is>
       </c>
       <c r="AY1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_GR_a_7</t>
+          <t>EDU</t>
         </is>
       </c>
       <c r="AZ1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_GR_a_9</t>
-        </is>
-      </c>
-      <c r="BA1" s="1" t="inlineStr">
-        <is>
-          <t>APP</t>
-        </is>
-      </c>
-      <c r="BB1" s="1" t="inlineStr">
-        <is>
-          <t>UX_A</t>
-        </is>
-      </c>
-      <c r="BC1" s="1" t="inlineStr">
-        <is>
-          <t>UX_P</t>
-        </is>
-      </c>
-      <c r="BD1" s="1" t="inlineStr">
-        <is>
-          <t>UX_E</t>
-        </is>
-      </c>
-      <c r="BE1" s="1" t="inlineStr">
-        <is>
-          <t>UX_D</t>
-        </is>
-      </c>
-      <c r="BF1" s="1" t="inlineStr">
-        <is>
-          <t>UX_S</t>
-        </is>
-      </c>
-      <c r="BG1" s="1" t="inlineStr">
-        <is>
-          <t>UX_N</t>
-        </is>
-      </c>
-      <c r="BH1" s="1" t="inlineStr">
-        <is>
-          <t>SUS</t>
-        </is>
-      </c>
-      <c r="BI1" s="1" t="inlineStr">
-        <is>
-          <t>CL_W_MD</t>
-        </is>
-      </c>
-      <c r="BJ1" s="1" t="inlineStr">
-        <is>
-          <t>CL_W_PD</t>
-        </is>
-      </c>
-      <c r="BK1" s="1" t="inlineStr">
-        <is>
-          <t>CL_W_TD</t>
-        </is>
-      </c>
-      <c r="BL1" s="1" t="inlineStr">
-        <is>
-          <t>CL_W_E</t>
-        </is>
-      </c>
-      <c r="BM1" s="1" t="inlineStr">
-        <is>
-          <t>CL_W_P</t>
-        </is>
-      </c>
-      <c r="BN1" s="1" t="inlineStr">
-        <is>
-          <t>CL_W_F</t>
-        </is>
-      </c>
-      <c r="BO1" s="1" t="inlineStr">
-        <is>
-          <t>CL_MD</t>
-        </is>
-      </c>
-      <c r="BP1" s="1" t="inlineStr">
-        <is>
-          <t>CL_PD</t>
-        </is>
-      </c>
-      <c r="BQ1" s="1" t="inlineStr">
-        <is>
-          <t>CL_TD</t>
-        </is>
-      </c>
-      <c r="BR1" s="1" t="inlineStr">
-        <is>
-          <t>CL_E</t>
-        </is>
-      </c>
-      <c r="BS1" s="1" t="inlineStr">
-        <is>
-          <t>CL_P</t>
-        </is>
-      </c>
-      <c r="BT1" s="1" t="inlineStr">
-        <is>
-          <t>CL_F</t>
-        </is>
-      </c>
-      <c r="BU1" s="1" t="inlineStr">
-        <is>
-          <t>CL_SCORE</t>
+          <t>VR_FREQUENCY</t>
         </is>
       </c>
     </row>
@@ -804,224 +699,161 @@
           <t>AA</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>TSV</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>QUEST</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>ALL</t>
         </is>
       </c>
+      <c r="D2" t="n">
+        <v>1433.02</v>
+      </c>
+      <c r="E2" t="n">
+        <v>24</v>
+      </c>
+      <c r="F2" t="n">
+        <v>52.486875</v>
+      </c>
       <c r="G2" t="n">
-        <v>1433.02</v>
+        <v>149</v>
       </c>
       <c r="H2" t="n">
+        <v>55</v>
+      </c>
+      <c r="I2" t="n">
+        <v>94</v>
+      </c>
+      <c r="J2" t="n">
+        <v>49</v>
+      </c>
+      <c r="K2" t="n">
+        <v>18</v>
+      </c>
+      <c r="L2" t="n">
+        <v>31</v>
+      </c>
+      <c r="M2" t="n">
+        <v>49</v>
+      </c>
+      <c r="N2" t="n">
+        <v>18</v>
+      </c>
+      <c r="O2" t="n">
+        <v>31</v>
+      </c>
+      <c r="P2" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>10</v>
+      </c>
+      <c r="R2" t="n">
+        <v>16</v>
+      </c>
+      <c r="S2" t="n">
+        <v>25</v>
+      </c>
+      <c r="T2" t="n">
+        <v>9</v>
+      </c>
+      <c r="U2" t="n">
+        <v>16</v>
+      </c>
+      <c r="V2" t="n">
+        <v>42</v>
+      </c>
+      <c r="W2" t="n">
+        <v>36</v>
+      </c>
+      <c r="X2" t="n">
         <v>24</v>
       </c>
-      <c r="I2" t="n">
-        <v>52.486875</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
-        <v>149</v>
-      </c>
-      <c r="L2" t="n">
-        <v>55</v>
-      </c>
-      <c r="M2" t="n">
-        <v>94</v>
-      </c>
-      <c r="N2" t="n">
-        <v>49</v>
-      </c>
-      <c r="O2" t="n">
-        <v>18</v>
-      </c>
-      <c r="P2" t="n">
-        <v>31</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>49</v>
-      </c>
-      <c r="R2" t="n">
-        <v>18</v>
-      </c>
-      <c r="S2" t="n">
-        <v>31</v>
-      </c>
-      <c r="T2" t="n">
-        <v>26</v>
-      </c>
-      <c r="U2" t="n">
-        <v>10</v>
-      </c>
-      <c r="V2" t="n">
-        <v>16</v>
-      </c>
-      <c r="W2" t="n">
-        <v>25</v>
-      </c>
-      <c r="X2" t="n">
-        <v>9</v>
-      </c>
       <c r="Y2" t="n">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="Z2" t="n">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="AA2" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="AB2" t="n">
-        <v>24</v>
+        <v>8.734</v>
       </c>
       <c r="AC2" t="n">
-        <v>33</v>
+        <v>18.014</v>
       </c>
       <c r="AD2" t="n">
-        <v>6</v>
+        <v>13.9</v>
       </c>
       <c r="AE2" t="n">
-        <v>6</v>
+        <v>0.29</v>
       </c>
       <c r="AF2" t="n">
-        <v>8.734</v>
+        <v>0.2462777777777778</v>
       </c>
       <c r="AG2" t="n">
-        <v>18.014</v>
+        <v>0.332741935483871</v>
       </c>
       <c r="AH2" t="n">
-        <v>13.9</v>
+        <v>19.885</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.29</v>
+        <v>15.22333333333333</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.2462777777777778</v>
+        <v>24.547625</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.332741935483871</v>
+        <v>0.213</v>
       </c>
       <c r="AL2" t="n">
-        <v>19.885</v>
+        <v>0.278</v>
       </c>
       <c r="AM2" t="n">
-        <v>15.22333333333333</v>
+        <v>0.28</v>
       </c>
       <c r="AN2" t="n">
-        <v>24.547625</v>
+        <v>0.363</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.213</v>
+        <v>0.528</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.278</v>
+        <v>0.451</v>
       </c>
       <c r="AQ2" t="n">
-        <v>0.28</v>
+        <v>5.343</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.363</v>
+        <v>16.415</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.528</v>
+        <v>60.143</v>
       </c>
       <c r="AT2" t="n">
-        <v>0.451</v>
+        <v>47.91</v>
       </c>
       <c r="AU2" t="n">
-        <v>5.343</v>
+        <v>1.872</v>
       </c>
       <c r="AV2" t="n">
-        <v>16.415</v>
+        <v>1.716</v>
       </c>
       <c r="AW2" t="n">
-        <v>60.143</v>
-      </c>
-      <c r="AX2" t="n">
-        <v>47.91</v>
-      </c>
-      <c r="AY2" t="n">
-        <v>1.872</v>
+        <v>21</v>
+      </c>
+      <c r="AX2" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="AY2" t="inlineStr">
+        <is>
+          <t>Grado universitario</t>
+        </is>
       </c>
       <c r="AZ2" t="n">
-        <v>1.716</v>
-      </c>
-      <c r="BA2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD2" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="BE2" t="n">
-        <v>-0.75</v>
-      </c>
-      <c r="BF2" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="BG2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="BH2" t="n">
-        <v>90</v>
-      </c>
-      <c r="BI2" t="n">
-        <v>0.133</v>
-      </c>
-      <c r="BJ2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="BK2" t="n">
-        <v>0.067</v>
-      </c>
-      <c r="BL2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="BM2" t="n">
-        <v>0.067</v>
-      </c>
-      <c r="BN2" t="n">
-        <v>0.333</v>
-      </c>
-      <c r="BO2" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="BP2" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="BQ2" t="n">
-        <v>0.133</v>
-      </c>
-      <c r="BR2" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="BS2" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="BT2" t="n">
-        <v>0.333</v>
-      </c>
-      <c r="BU2" t="n">
-        <v>4.666</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -1033,228 +865,165 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>CTRL</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>QUEST</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>ALL</t>
         </is>
       </c>
+      <c r="D3" t="n">
+        <v>1236.99</v>
+      </c>
+      <c r="E3" t="n">
+        <v>24</v>
+      </c>
+      <c r="F3" t="n">
+        <v>43.423375</v>
+      </c>
       <c r="G3" t="n">
-        <v>1236.99</v>
+        <v>146</v>
       </c>
       <c r="H3" t="n">
+        <v>112</v>
+      </c>
+      <c r="I3" t="n">
+        <v>34</v>
+      </c>
+      <c r="J3" t="n">
+        <v>43</v>
+      </c>
+      <c r="K3" t="n">
+        <v>32</v>
+      </c>
+      <c r="L3" t="n">
+        <v>11</v>
+      </c>
+      <c r="M3" t="n">
+        <v>43</v>
+      </c>
+      <c r="N3" t="n">
+        <v>32</v>
+      </c>
+      <c r="O3" t="n">
+        <v>11</v>
+      </c>
+      <c r="P3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q3" t="n">
         <v>24</v>
       </c>
-      <c r="I3" t="n">
-        <v>43.423375</v>
-      </c>
-      <c r="J3" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" t="n">
-        <v>146</v>
-      </c>
-      <c r="L3" t="n">
-        <v>112</v>
-      </c>
-      <c r="M3" t="n">
-        <v>34</v>
-      </c>
-      <c r="N3" t="n">
-        <v>43</v>
-      </c>
-      <c r="O3" t="n">
-        <v>32</v>
-      </c>
-      <c r="P3" t="n">
-        <v>11</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>43</v>
-      </c>
       <c r="R3" t="n">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="S3" t="n">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="T3" t="n">
+        <v>24</v>
+      </c>
+      <c r="U3" t="n">
+        <v>6</v>
+      </c>
+      <c r="V3" t="n">
+        <v>42</v>
+      </c>
+      <c r="W3" t="n">
+        <v>36</v>
+      </c>
+      <c r="X3" t="n">
         <v>30</v>
       </c>
-      <c r="U3" t="n">
+      <c r="Y3" t="n">
+        <v>14</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="n">
         <v>24</v>
       </c>
-      <c r="V3" t="n">
-        <v>6</v>
-      </c>
-      <c r="W3" t="n">
-        <v>30</v>
-      </c>
-      <c r="X3" t="n">
-        <v>24</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>6</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>42</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>36</v>
-      </c>
       <c r="AB3" t="n">
-        <v>30</v>
+        <v>7.745</v>
       </c>
       <c r="AC3" t="n">
-        <v>14</v>
+        <v>10.082</v>
       </c>
       <c r="AD3" t="n">
-        <v>0</v>
+        <v>34.031</v>
       </c>
       <c r="AE3" t="n">
-        <v>24</v>
+        <v>0.367</v>
       </c>
       <c r="AF3" t="n">
-        <v>7.745</v>
+        <v>0.22934375</v>
       </c>
       <c r="AG3" t="n">
-        <v>10.082</v>
+        <v>0.505</v>
       </c>
       <c r="AH3" t="n">
-        <v>34.031</v>
+        <v>33.431</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.367</v>
+        <v>12.91883333333333</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.22934375</v>
+        <v>53.943</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.505</v>
+        <v>0.454</v>
       </c>
       <c r="AL3" t="n">
-        <v>33.431</v>
+        <v>0.237</v>
       </c>
       <c r="AM3" t="n">
-        <v>12.91883333333333</v>
+        <v>0.266</v>
       </c>
       <c r="AN3" t="n">
-        <v>53.943</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>0.454</v>
+        <v>0.279</v>
+      </c>
+      <c r="AO3" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
       </c>
       <c r="AP3" t="n">
         <v>0.237</v>
       </c>
       <c r="AQ3" t="n">
-        <v>0.266</v>
+        <v>3.752</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.279</v>
-      </c>
-      <c r="AS3" t="inlineStr">
+        <v>8.432</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>157.554</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>54.786</v>
+      </c>
+      <c r="AU3" t="inlineStr">
         <is>
           <t>NULL</t>
         </is>
       </c>
-      <c r="AT3" t="n">
-        <v>0.237</v>
-      </c>
-      <c r="AU3" t="n">
-        <v>3.752</v>
-      </c>
       <c r="AV3" t="n">
-        <v>8.432</v>
+        <v>0.961</v>
       </c>
       <c r="AW3" t="n">
-        <v>157.554</v>
-      </c>
-      <c r="AX3" t="n">
-        <v>54.786</v>
+        <v>21</v>
+      </c>
+      <c r="AX3" t="inlineStr">
+        <is>
+          <t>NB</t>
+        </is>
       </c>
       <c r="AY3" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Grado universitario</t>
         </is>
       </c>
       <c r="AZ3" t="n">
-        <v>0.961</v>
-      </c>
-      <c r="BA3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB3" t="n">
-        <v>-0.333</v>
-      </c>
-      <c r="BC3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD3" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="BE3" t="n">
-        <v>-0.25</v>
-      </c>
-      <c r="BF3" t="n">
-        <v>-1</v>
-      </c>
-      <c r="BG3" t="n">
-        <v>-0.25</v>
-      </c>
-      <c r="BH3" t="n">
-        <v>92.5</v>
-      </c>
-      <c r="BI3" t="n">
-        <v>0.333</v>
-      </c>
-      <c r="BJ3" t="n">
-        <v>0.067</v>
-      </c>
-      <c r="BK3" t="n">
-        <v>0.133</v>
-      </c>
-      <c r="BL3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="BM3" t="n">
-        <v>0.267</v>
-      </c>
-      <c r="BN3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BO3" t="n">
-        <v>0.333</v>
-      </c>
-      <c r="BP3" t="n">
-        <v>0.067</v>
-      </c>
-      <c r="BQ3" t="n">
-        <v>0.133</v>
-      </c>
-      <c r="BR3" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="BS3" t="n">
-        <v>2.133</v>
-      </c>
-      <c r="BT3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BU3" t="n">
-        <v>4.066</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creo que he terminado con el analisis del cuestionario. Ahora estaba con las tablas combinadas. Por ejemplo, número de interacciones / tareas realizadas, tiempo desde que se inicia la tarea hasta que se interactua por primera vez...
</commit_message>
<xml_diff>
--- a/data_analysis/db_env/app/results/resultsALL.xlsx
+++ b/data_analysis/db_env/app/results/resultsALL.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AZ3"/>
+  <dimension ref="A1:DF3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,252 +441,542 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>AGE</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>GENRE</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>EDU</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>VR_FREQUENCY</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>EX_PRE_1</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>EX_PRE_2</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>EX_PRE_3</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>EX_PRE_4_0</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>EX_PRE_4_1</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>EX_PRE_4_2</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>EX_PRE_4_3</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>EX_PRE_5</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>EX_PRE_6</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>EX_PRE_7</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>EX_PRE_8_0</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>EX_PRE_8_1</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>EX_PRE_8_2</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>EX_PRE_8_3</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>EX_PRE_9</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>EX_PRE_10</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>EX_PRE_11</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>EX_PRE_12</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>EX_PRE_SCORE</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>UX_A</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>UX_P</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>UX_E</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>UX_D</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>UX_S</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>UX_N</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>SUS</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>CL_W_MD</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>CL_W_PD</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>CL_W_TD</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>CL_W_E</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>CL_W_P</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>CL_W_F</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>CL_MD</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>CL_PD</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>CL_TD</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>CL_E</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>CL_P</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>CL_F</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>CL_SCORE</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>EX_POST_1</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>EX_POST_2</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>EX_POST_3</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>EX_POST_4_0</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>EX_POST_4_1</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>EX_POST_4_2</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>EX_POST_4_3</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>EX_POST_5</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>EX_POST_6</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>EX_POST_7</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>EX_POST_8_0</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>EX_POST_8_1</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>EX_POST_8_2</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>EX_POST_8_3</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>EX_POST_9</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>EX_POST_10</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>EX_POST_11</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>EX_POST_12</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>EX_POST_SCORE</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
           <t>SCENARIO</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="BN1" s="1" t="inlineStr">
         <is>
           <t>TD</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="BO1" s="1" t="inlineStr">
         <is>
           <t>GP_N</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="BP1" s="1" t="inlineStr">
         <is>
           <t>GP_T</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="BQ1" s="1" t="inlineStr">
         <is>
           <t>OI_N</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="BR1" s="1" t="inlineStr">
         <is>
           <t>OI_N_R</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="BS1" s="1" t="inlineStr">
         <is>
           <t>OI_N_L</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="BT1" s="1" t="inlineStr">
         <is>
           <t>OI_N_t_1</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="BU1" s="1" t="inlineStr">
         <is>
           <t>OI_N_t_1_R</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="BV1" s="1" t="inlineStr">
         <is>
           <t>OI_N_t_1_L</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="BW1" s="1" t="inlineStr">
         <is>
           <t>OI_N_t_2</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="BX1" s="1" t="inlineStr">
         <is>
           <t>OI_N_t_2_R</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="BY1" s="1" t="inlineStr">
         <is>
           <t>OI_N_t_2_L</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="BZ1" s="1" t="inlineStr">
         <is>
           <t>OI_N_t_3</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="CA1" s="1" t="inlineStr">
         <is>
           <t>OI_N_t_3_R</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="CB1" s="1" t="inlineStr">
         <is>
           <t>OI_N_t_3_L</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="CC1" s="1" t="inlineStr">
         <is>
           <t>OI_N_t_4</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="CD1" s="1" t="inlineStr">
         <is>
           <t>OI_N_t_4_R</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="CE1" s="1" t="inlineStr">
         <is>
           <t>OI_N_t_4_L</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="CF1" s="1" t="inlineStr">
         <is>
           <t>OI_N_a_2</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="CG1" s="1" t="inlineStr">
         <is>
           <t>OI_N_a_3</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="CH1" s="1" t="inlineStr">
         <is>
           <t>OI_N_a_4</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="CI1" s="1" t="inlineStr">
         <is>
           <t>OI_N_a_5</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="CJ1" s="1" t="inlineStr">
         <is>
           <t>OI_N_a_7</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="CK1" s="1" t="inlineStr">
         <is>
           <t>OI_N_a_9</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="CL1" s="1" t="inlineStr">
         <is>
           <t>OI_T</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="CM1" s="1" t="inlineStr">
         <is>
           <t>OI_T_R</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="CN1" s="1" t="inlineStr">
         <is>
           <t>OI_T_L</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="CO1" s="1" t="inlineStr">
         <is>
           <t>OI_T_SS</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="CP1" s="1" t="inlineStr">
         <is>
           <t>OI_T_SS_R</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="CQ1" s="1" t="inlineStr">
         <is>
           <t>OI_T_SS_L</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="CR1" s="1" t="inlineStr">
         <is>
           <t>OI_T_GR</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="CS1" s="1" t="inlineStr">
         <is>
           <t>OI_T_GR_R</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="CT1" s="1" t="inlineStr">
         <is>
           <t>OI_T_GR_L</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="CU1" s="1" t="inlineStr">
         <is>
           <t>OI_T_SS_a_2</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="CV1" s="1" t="inlineStr">
         <is>
           <t>OI_T_SS_a_3</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="CW1" s="1" t="inlineStr">
         <is>
           <t>OI_T_SS_a_4</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="CX1" s="1" t="inlineStr">
         <is>
           <t>OI_T_SS_a_5</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="CY1" s="1" t="inlineStr">
         <is>
           <t>OI_T_SS_a_7</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="CZ1" s="1" t="inlineStr">
         <is>
           <t>OI_T_SS_a_9</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="DA1" s="1" t="inlineStr">
         <is>
           <t>OI_T_GR_a_2</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="DB1" s="1" t="inlineStr">
         <is>
           <t>OI_T_GR_a_3</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="DC1" s="1" t="inlineStr">
         <is>
           <t>OI_T_GR_a_4</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="DD1" s="1" t="inlineStr">
         <is>
           <t>OI_T_GR_a_5</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="DE1" s="1" t="inlineStr">
         <is>
           <t>OI_T_GR_a_7</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="DF1" s="1" t="inlineStr">
         <is>
           <t>OI_T_GR_a_9</t>
-        </is>
-      </c>
-      <c r="AW1" s="1" t="inlineStr">
-        <is>
-          <t>AGE</t>
-        </is>
-      </c>
-      <c r="AX1" s="1" t="inlineStr">
-        <is>
-          <t>GENRE</t>
-        </is>
-      </c>
-      <c r="AY1" s="1" t="inlineStr">
-        <is>
-          <t>EDU</t>
-        </is>
-      </c>
-      <c r="AZ1" s="1" t="inlineStr">
-        <is>
-          <t>VR_FREQUENCY</t>
         </is>
       </c>
     </row>
@@ -699,161 +989,375 @@
           <t>AA</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="n">
+        <v>21</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Grado universitario</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>la mano derecha</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>La sonda SABG-100 …</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Un dosímetro personal electrónico (EPD) …</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>En el suelo aparece un círculo con el objeto flotando alrededor.</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>Al acercar la mano al objeto, la mano vibra y se pone de color azul</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>Se pueden sacar varias al mismo tiempo</t>
+        </is>
+      </c>
+      <c r="Y2" t="n">
+        <v>9</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>-0.75</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>90</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.067</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.067</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>4.666</v>
+      </c>
+      <c r="AT2" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="AU2" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="AV2" t="inlineStr">
+        <is>
+          <t>la mano derecha</t>
+        </is>
+      </c>
+      <c r="AW2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA2" t="inlineStr">
+        <is>
+          <t>La sonda SABG-100 …</t>
+        </is>
+      </c>
+      <c r="BB2" t="inlineStr">
+        <is>
+          <t>Un dosímetro personal electrónico (EPD) …</t>
+        </is>
+      </c>
+      <c r="BC2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="BD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH2" t="inlineStr">
+        <is>
+          <t>En el suelo, aparece un círculo con el objeto flotando alrededor.</t>
+        </is>
+      </c>
+      <c r="BI2" t="inlineStr">
+        <is>
+          <t>Al acercar la mano al objeto, la mano vibra y se pone de color azul</t>
+        </is>
+      </c>
+      <c r="BJ2" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="BK2" t="inlineStr">
+        <is>
+          <t>Se pueden sacar varias al mismo tiempo</t>
+        </is>
+      </c>
+      <c r="BL2" t="n">
+        <v>9</v>
+      </c>
+      <c r="BM2" t="inlineStr">
         <is>
           <t>ALL</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="BN2" t="n">
         <v>1433.02</v>
       </c>
-      <c r="E2" t="n">
+      <c r="BO2" t="n">
         <v>24</v>
       </c>
-      <c r="F2" t="n">
+      <c r="BP2" t="n">
         <v>52.486875</v>
       </c>
-      <c r="G2" t="n">
+      <c r="BQ2" t="n">
         <v>149</v>
       </c>
-      <c r="H2" t="n">
+      <c r="BR2" t="n">
         <v>55</v>
       </c>
-      <c r="I2" t="n">
+      <c r="BS2" t="n">
         <v>94</v>
       </c>
-      <c r="J2" t="n">
+      <c r="BT2" t="n">
         <v>49</v>
       </c>
-      <c r="K2" t="n">
+      <c r="BU2" t="n">
         <v>18</v>
       </c>
-      <c r="L2" t="n">
+      <c r="BV2" t="n">
         <v>31</v>
       </c>
-      <c r="M2" t="n">
+      <c r="BW2" t="n">
         <v>49</v>
       </c>
-      <c r="N2" t="n">
+      <c r="BX2" t="n">
         <v>18</v>
       </c>
-      <c r="O2" t="n">
+      <c r="BY2" t="n">
         <v>31</v>
       </c>
-      <c r="P2" t="n">
+      <c r="BZ2" t="n">
         <v>26</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="CA2" t="n">
         <v>10</v>
       </c>
-      <c r="R2" t="n">
+      <c r="CB2" t="n">
         <v>16</v>
       </c>
-      <c r="S2" t="n">
+      <c r="CC2" t="n">
         <v>25</v>
       </c>
-      <c r="T2" t="n">
+      <c r="CD2" t="n">
         <v>9</v>
       </c>
-      <c r="U2" t="n">
+      <c r="CE2" t="n">
         <v>16</v>
       </c>
-      <c r="V2" t="n">
+      <c r="CF2" t="n">
         <v>42</v>
       </c>
-      <c r="W2" t="n">
+      <c r="CG2" t="n">
         <v>36</v>
       </c>
-      <c r="X2" t="n">
+      <c r="CH2" t="n">
         <v>24</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="CI2" t="n">
         <v>33</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="CJ2" t="n">
         <v>6</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="CK2" t="n">
         <v>6</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="CL2" t="n">
         <v>8.734</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="CM2" t="n">
         <v>18.014</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="CN2" t="n">
         <v>13.9</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="CO2" t="n">
         <v>0.29</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="CP2" t="n">
         <v>0.2462777777777778</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="CQ2" t="n">
         <v>0.332741935483871</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="CR2" t="n">
         <v>19.885</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="CS2" t="n">
         <v>15.22333333333333</v>
       </c>
-      <c r="AJ2" t="n">
+      <c r="CT2" t="n">
         <v>24.547625</v>
       </c>
-      <c r="AK2" t="n">
+      <c r="CU2" t="n">
         <v>0.213</v>
       </c>
-      <c r="AL2" t="n">
+      <c r="CV2" t="n">
         <v>0.278</v>
       </c>
-      <c r="AM2" t="n">
+      <c r="CW2" t="n">
         <v>0.28</v>
       </c>
-      <c r="AN2" t="n">
+      <c r="CX2" t="n">
         <v>0.363</v>
       </c>
-      <c r="AO2" t="n">
+      <c r="CY2" t="n">
         <v>0.528</v>
       </c>
-      <c r="AP2" t="n">
+      <c r="CZ2" t="n">
         <v>0.451</v>
       </c>
-      <c r="AQ2" t="n">
+      <c r="DA2" t="n">
         <v>5.343</v>
       </c>
-      <c r="AR2" t="n">
+      <c r="DB2" t="n">
         <v>16.415</v>
       </c>
-      <c r="AS2" t="n">
+      <c r="DC2" t="n">
         <v>60.143</v>
       </c>
-      <c r="AT2" t="n">
+      <c r="DD2" t="n">
         <v>47.91</v>
       </c>
-      <c r="AU2" t="n">
+      <c r="DE2" t="n">
         <v>1.872</v>
       </c>
-      <c r="AV2" t="n">
+      <c r="DF2" t="n">
         <v>1.716</v>
-      </c>
-      <c r="AW2" t="n">
-        <v>21</v>
-      </c>
-      <c r="AX2" t="inlineStr">
-        <is>
-          <t>H</t>
-        </is>
-      </c>
-      <c r="AY2" t="inlineStr">
-        <is>
-          <t>Grado universitario</t>
-        </is>
-      </c>
-      <c r="AZ2" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -865,165 +1369,379 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" t="n">
+        <v>21</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NB</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Grado universitario</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Ninguna de las anteriores</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>la mano derecha</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>La sonda SABG-100 …</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Un dosímetro personal electrónico (EPD) …</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>En el suelo aparece un círculo con el objeto flotando alrededor.</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Al acercar la mano al objeto, la mano vibra y se pone de color verde</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>Se pueden sacar varias al mismo tiempo</t>
+        </is>
+      </c>
+      <c r="Y3" t="n">
+        <v>11</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>-0.333</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>92.5</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0.067</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>0.267</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>0.067</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>2.133</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>4.066</v>
+      </c>
+      <c r="AT3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="AU3" t="inlineStr">
+        <is>
+          <t>Ninguna de las anteriores</t>
+        </is>
+      </c>
+      <c r="AV3" t="inlineStr">
+        <is>
+          <t>la mano derecha</t>
+        </is>
+      </c>
+      <c r="AW3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA3" t="inlineStr">
+        <is>
+          <t>La sonda SABG-100 …</t>
+        </is>
+      </c>
+      <c r="BB3" t="inlineStr">
+        <is>
+          <t>Un dosímetro personal electrónico (EPD) …</t>
+        </is>
+      </c>
+      <c r="BC3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="BD3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH3" t="inlineStr">
+        <is>
+          <t>En el suelo, aparece un círculo con el objeto flotando alrededor.</t>
+        </is>
+      </c>
+      <c r="BI3" t="inlineStr">
+        <is>
+          <t>Al acercar la mano al objeto, la mano vibra y se pone de color verde</t>
+        </is>
+      </c>
+      <c r="BJ3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="BK3" t="inlineStr">
+        <is>
+          <t>Se pueden sacar varias al mismo tiempo</t>
+        </is>
+      </c>
+      <c r="BL3" t="n">
+        <v>11</v>
+      </c>
+      <c r="BM3" t="inlineStr">
         <is>
           <t>ALL</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="BN3" t="n">
         <v>1236.99</v>
       </c>
-      <c r="E3" t="n">
+      <c r="BO3" t="n">
         <v>24</v>
       </c>
-      <c r="F3" t="n">
+      <c r="BP3" t="n">
         <v>43.423375</v>
       </c>
-      <c r="G3" t="n">
+      <c r="BQ3" t="n">
         <v>146</v>
       </c>
-      <c r="H3" t="n">
+      <c r="BR3" t="n">
         <v>112</v>
       </c>
-      <c r="I3" t="n">
+      <c r="BS3" t="n">
         <v>34</v>
       </c>
-      <c r="J3" t="n">
+      <c r="BT3" t="n">
         <v>43</v>
       </c>
-      <c r="K3" t="n">
+      <c r="BU3" t="n">
         <v>32</v>
       </c>
-      <c r="L3" t="n">
+      <c r="BV3" t="n">
         <v>11</v>
       </c>
-      <c r="M3" t="n">
+      <c r="BW3" t="n">
         <v>43</v>
       </c>
-      <c r="N3" t="n">
+      <c r="BX3" t="n">
         <v>32</v>
       </c>
-      <c r="O3" t="n">
+      <c r="BY3" t="n">
         <v>11</v>
       </c>
-      <c r="P3" t="n">
+      <c r="BZ3" t="n">
         <v>30</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="CA3" t="n">
         <v>24</v>
       </c>
-      <c r="R3" t="n">
+      <c r="CB3" t="n">
         <v>6</v>
       </c>
-      <c r="S3" t="n">
+      <c r="CC3" t="n">
         <v>30</v>
       </c>
-      <c r="T3" t="n">
+      <c r="CD3" t="n">
         <v>24</v>
       </c>
-      <c r="U3" t="n">
+      <c r="CE3" t="n">
         <v>6</v>
       </c>
-      <c r="V3" t="n">
+      <c r="CF3" t="n">
         <v>42</v>
       </c>
-      <c r="W3" t="n">
+      <c r="CG3" t="n">
         <v>36</v>
       </c>
-      <c r="X3" t="n">
+      <c r="CH3" t="n">
         <v>30</v>
       </c>
-      <c r="Y3" t="n">
+      <c r="CI3" t="n">
         <v>14</v>
       </c>
-      <c r="Z3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA3" t="n">
+      <c r="CJ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CK3" t="n">
         <v>24</v>
       </c>
-      <c r="AB3" t="n">
+      <c r="CL3" t="n">
         <v>7.745</v>
       </c>
-      <c r="AC3" t="n">
+      <c r="CM3" t="n">
         <v>10.082</v>
       </c>
-      <c r="AD3" t="n">
+      <c r="CN3" t="n">
         <v>34.031</v>
       </c>
-      <c r="AE3" t="n">
+      <c r="CO3" t="n">
         <v>0.367</v>
       </c>
-      <c r="AF3" t="n">
+      <c r="CP3" t="n">
         <v>0.22934375</v>
       </c>
-      <c r="AG3" t="n">
+      <c r="CQ3" t="n">
         <v>0.505</v>
       </c>
-      <c r="AH3" t="n">
+      <c r="CR3" t="n">
         <v>33.431</v>
       </c>
-      <c r="AI3" t="n">
+      <c r="CS3" t="n">
         <v>12.91883333333333</v>
       </c>
-      <c r="AJ3" t="n">
+      <c r="CT3" t="n">
         <v>53.943</v>
       </c>
-      <c r="AK3" t="n">
+      <c r="CU3" t="n">
         <v>0.454</v>
       </c>
-      <c r="AL3" t="n">
+      <c r="CV3" t="n">
         <v>0.237</v>
       </c>
-      <c r="AM3" t="n">
+      <c r="CW3" t="n">
         <v>0.266</v>
       </c>
-      <c r="AN3" t="n">
+      <c r="CX3" t="n">
         <v>0.279</v>
       </c>
-      <c r="AO3" t="inlineStr">
+      <c r="CY3" t="inlineStr">
         <is>
           <t>NULL</t>
         </is>
       </c>
-      <c r="AP3" t="n">
+      <c r="CZ3" t="n">
         <v>0.237</v>
       </c>
-      <c r="AQ3" t="n">
+      <c r="DA3" t="n">
         <v>3.752</v>
       </c>
-      <c r="AR3" t="n">
+      <c r="DB3" t="n">
         <v>8.432</v>
       </c>
-      <c r="AS3" t="n">
+      <c r="DC3" t="n">
         <v>157.554</v>
       </c>
-      <c r="AT3" t="n">
+      <c r="DD3" t="n">
         <v>54.786</v>
       </c>
-      <c r="AU3" t="inlineStr">
+      <c r="DE3" t="inlineStr">
         <is>
           <t>NULL</t>
         </is>
       </c>
-      <c r="AV3" t="n">
+      <c r="DF3" t="n">
         <v>0.961</v>
-      </c>
-      <c r="AW3" t="n">
-        <v>21</v>
-      </c>
-      <c r="AX3" t="inlineStr">
-        <is>
-          <t>NB</t>
-        </is>
-      </c>
-      <c r="AY3" t="inlineStr">
-        <is>
-          <t>Grado universitario</t>
-        </is>
-      </c>
-      <c r="AZ3" t="n">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Estaba con los eventos del HelpPanel
</commit_message>
<xml_diff>
--- a/data_analysis/db_env/app/results/resultsALL.xlsx
+++ b/data_analysis/db_env/app/results/resultsALL.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DF3"/>
+  <dimension ref="A1:DD3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -756,227 +756,217 @@
       </c>
       <c r="BN1" s="1" t="inlineStr">
         <is>
-          <t>TD</t>
+          <t>OI_N</t>
         </is>
       </c>
       <c r="BO1" s="1" t="inlineStr">
         <is>
-          <t>GP_N</t>
+          <t>OI_N_R</t>
         </is>
       </c>
       <c r="BP1" s="1" t="inlineStr">
         <is>
-          <t>GP_T</t>
+          <t>OI_N_L</t>
         </is>
       </c>
       <c r="BQ1" s="1" t="inlineStr">
         <is>
-          <t>OI_N</t>
+          <t>OI_N_t_1</t>
         </is>
       </c>
       <c r="BR1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_R</t>
+          <t>OI_N_t_1_R</t>
         </is>
       </c>
       <c r="BS1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_L</t>
+          <t>OI_N_t_1_L</t>
         </is>
       </c>
       <c r="BT1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_1</t>
+          <t>OI_N_t_2</t>
         </is>
       </c>
       <c r="BU1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_1_R</t>
+          <t>OI_N_t_2_R</t>
         </is>
       </c>
       <c r="BV1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_1_L</t>
+          <t>OI_N_t_2_L</t>
         </is>
       </c>
       <c r="BW1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_2</t>
+          <t>OI_N_t_3</t>
         </is>
       </c>
       <c r="BX1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_2_R</t>
+          <t>OI_N_t_3_R</t>
         </is>
       </c>
       <c r="BY1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_2_L</t>
+          <t>OI_N_t_3_L</t>
         </is>
       </c>
       <c r="BZ1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_3</t>
+          <t>OI_N_t_4</t>
         </is>
       </c>
       <c r="CA1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_3_R</t>
+          <t>OI_N_t_4_R</t>
         </is>
       </c>
       <c r="CB1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_3_L</t>
+          <t>OI_N_t_4_L</t>
         </is>
       </c>
       <c r="CC1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_4</t>
+          <t>OI_N_a_2</t>
         </is>
       </c>
       <c r="CD1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_4_R</t>
+          <t>OI_N_a_3</t>
         </is>
       </c>
       <c r="CE1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_t_4_L</t>
+          <t>OI_N_a_4</t>
         </is>
       </c>
       <c r="CF1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_a_2</t>
+          <t>OI_N_a_5</t>
         </is>
       </c>
       <c r="CG1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_a_3</t>
+          <t>OI_N_a_7</t>
         </is>
       </c>
       <c r="CH1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_a_4</t>
+          <t>OI_N_a_9</t>
         </is>
       </c>
       <c r="CI1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_a_5</t>
+          <t>OI_T</t>
         </is>
       </c>
       <c r="CJ1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_a_7</t>
+          <t>OI_T_R</t>
         </is>
       </c>
       <c r="CK1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_a_9</t>
+          <t>OI_T_L</t>
         </is>
       </c>
       <c r="CL1" s="1" t="inlineStr">
         <is>
-          <t>OI_T</t>
+          <t>OI_T_SS</t>
         </is>
       </c>
       <c r="CM1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_R</t>
+          <t>OI_T_SS_R</t>
         </is>
       </c>
       <c r="CN1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_L</t>
+          <t>OI_T_SS_L</t>
         </is>
       </c>
       <c r="CO1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_SS</t>
+          <t>OI_T_GR</t>
         </is>
       </c>
       <c r="CP1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_SS_R</t>
+          <t>OI_T_GR_R</t>
         </is>
       </c>
       <c r="CQ1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_SS_L</t>
+          <t>OI_T_GR_L</t>
         </is>
       </c>
       <c r="CR1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_GR</t>
+          <t>OI_T_SS_a_2</t>
         </is>
       </c>
       <c r="CS1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_GR_R</t>
+          <t>OI_T_SS_a_3</t>
         </is>
       </c>
       <c r="CT1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_GR_L</t>
+          <t>OI_T_SS_a_4</t>
         </is>
       </c>
       <c r="CU1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_SS_a_2</t>
+          <t>OI_T_SS_a_5</t>
         </is>
       </c>
       <c r="CV1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_SS_a_3</t>
+          <t>OI_T_SS_a_7</t>
         </is>
       </c>
       <c r="CW1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_SS_a_4</t>
+          <t>OI_T_SS_a_9</t>
         </is>
       </c>
       <c r="CX1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_SS_a_5</t>
+          <t>OI_T_GR_a_2</t>
         </is>
       </c>
       <c r="CY1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_SS_a_7</t>
+          <t>OI_T_GR_a_3</t>
         </is>
       </c>
       <c r="CZ1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_SS_a_9</t>
+          <t>OI_T_GR_a_4</t>
         </is>
       </c>
       <c r="DA1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_GR_a_2</t>
+          <t>OI_T_GR_a_5</t>
         </is>
       </c>
       <c r="DB1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_GR_a_3</t>
+          <t>OI_T_GR_a_7</t>
         </is>
       </c>
       <c r="DC1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_GR_a_4</t>
+          <t>OI_T_GR_a_9</t>
         </is>
       </c>
       <c r="DD1" s="1" t="inlineStr">
         <is>
-          <t>OI_T_GR_a_5</t>
-        </is>
-      </c>
-      <c r="DE1" s="1" t="inlineStr">
-        <is>
-          <t>OI_T_GR_a_7</t>
-        </is>
-      </c>
-      <c r="DF1" s="1" t="inlineStr">
-        <is>
-          <t>OI_T_GR_a_9</t>
+          <t>OI_T_EPD</t>
         </is>
       </c>
     </row>
@@ -1225,22 +1215,22 @@
         </is>
       </c>
       <c r="BN2" t="n">
-        <v>1433.02</v>
+        <v>149</v>
       </c>
       <c r="BO2" t="n">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="BP2" t="n">
-        <v>52.486875</v>
+        <v>94</v>
       </c>
       <c r="BQ2" t="n">
-        <v>149</v>
+        <v>49</v>
       </c>
       <c r="BR2" t="n">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="BS2" t="n">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="BT2" t="n">
         <v>49</v>
@@ -1252,112 +1242,106 @@
         <v>31</v>
       </c>
       <c r="BW2" t="n">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="BX2" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="BY2" t="n">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="BZ2" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="CA2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="CB2" t="n">
         <v>16</v>
       </c>
       <c r="CC2" t="n">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="CD2" t="n">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="CE2" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="CF2" t="n">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="CG2" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="CH2" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="CI2" t="n">
-        <v>33</v>
+        <v>8.734</v>
       </c>
       <c r="CJ2" t="n">
-        <v>6</v>
+        <v>18.014</v>
       </c>
       <c r="CK2" t="n">
-        <v>6</v>
+        <v>13.9</v>
       </c>
       <c r="CL2" t="n">
-        <v>8.734</v>
+        <v>0.29</v>
       </c>
       <c r="CM2" t="n">
-        <v>18.014</v>
+        <v>0.2462777777777778</v>
       </c>
       <c r="CN2" t="n">
-        <v>13.9</v>
+        <v>0.332741935483871</v>
       </c>
       <c r="CO2" t="n">
-        <v>0.29</v>
+        <v>19.885</v>
       </c>
       <c r="CP2" t="n">
-        <v>0.2462777777777778</v>
+        <v>15.22333333333333</v>
       </c>
       <c r="CQ2" t="n">
-        <v>0.332741935483871</v>
+        <v>24.547625</v>
       </c>
       <c r="CR2" t="n">
-        <v>19.885</v>
+        <v>0.213</v>
       </c>
       <c r="CS2" t="n">
-        <v>15.22333333333333</v>
+        <v>0.278</v>
       </c>
       <c r="CT2" t="n">
-        <v>24.547625</v>
+        <v>0.28</v>
       </c>
       <c r="CU2" t="n">
-        <v>0.213</v>
+        <v>0.363</v>
       </c>
       <c r="CV2" t="n">
-        <v>0.278</v>
+        <v>0.528</v>
       </c>
       <c r="CW2" t="n">
-        <v>0.28</v>
+        <v>0.451</v>
       </c>
       <c r="CX2" t="n">
-        <v>0.363</v>
+        <v>5.343</v>
       </c>
       <c r="CY2" t="n">
-        <v>0.528</v>
+        <v>16.415</v>
       </c>
       <c r="CZ2" t="n">
-        <v>0.451</v>
+        <v>60.143</v>
       </c>
       <c r="DA2" t="n">
-        <v>5.343</v>
+        <v>47.91</v>
       </c>
       <c r="DB2" t="n">
-        <v>16.415</v>
+        <v>1.872</v>
       </c>
       <c r="DC2" t="n">
-        <v>60.143</v>
+        <v>1.716</v>
       </c>
       <c r="DD2" t="n">
-        <v>47.91</v>
-      </c>
-      <c r="DE2" t="n">
-        <v>1.872</v>
-      </c>
-      <c r="DF2" t="n">
-        <v>1.716</v>
+        <v>249.672</v>
       </c>
     </row>
     <row r="3">
@@ -1605,22 +1589,22 @@
         </is>
       </c>
       <c r="BN3" t="n">
-        <v>1236.99</v>
+        <v>146</v>
       </c>
       <c r="BO3" t="n">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="BP3" t="n">
-        <v>43.423375</v>
+        <v>34</v>
       </c>
       <c r="BQ3" t="n">
-        <v>146</v>
+        <v>43</v>
       </c>
       <c r="BR3" t="n">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="BS3" t="n">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="BT3" t="n">
         <v>43</v>
@@ -1632,13 +1616,13 @@
         <v>11</v>
       </c>
       <c r="BW3" t="n">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="BX3" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="BY3" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="BZ3" t="n">
         <v>30</v>
@@ -1650,98 +1634,92 @@
         <v>6</v>
       </c>
       <c r="CC3" t="n">
+        <v>42</v>
+      </c>
+      <c r="CD3" t="n">
+        <v>36</v>
+      </c>
+      <c r="CE3" t="n">
         <v>30</v>
       </c>
-      <c r="CD3" t="n">
+      <c r="CF3" t="n">
+        <v>14</v>
+      </c>
+      <c r="CG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CH3" t="n">
         <v>24</v>
       </c>
-      <c r="CE3" t="n">
-        <v>6</v>
-      </c>
-      <c r="CF3" t="n">
-        <v>42</v>
-      </c>
-      <c r="CG3" t="n">
-        <v>36</v>
-      </c>
-      <c r="CH3" t="n">
-        <v>30</v>
-      </c>
       <c r="CI3" t="n">
-        <v>14</v>
+        <v>7.745</v>
       </c>
       <c r="CJ3" t="n">
-        <v>0</v>
+        <v>10.082</v>
       </c>
       <c r="CK3" t="n">
-        <v>24</v>
+        <v>34.031</v>
       </c>
       <c r="CL3" t="n">
-        <v>7.745</v>
+        <v>0.367</v>
       </c>
       <c r="CM3" t="n">
-        <v>10.082</v>
+        <v>0.22934375</v>
       </c>
       <c r="CN3" t="n">
-        <v>34.031</v>
+        <v>0.505</v>
       </c>
       <c r="CO3" t="n">
-        <v>0.367</v>
+        <v>33.431</v>
       </c>
       <c r="CP3" t="n">
-        <v>0.22934375</v>
+        <v>12.91883333333333</v>
       </c>
       <c r="CQ3" t="n">
-        <v>0.505</v>
+        <v>53.943</v>
       </c>
       <c r="CR3" t="n">
-        <v>33.431</v>
+        <v>0.454</v>
       </c>
       <c r="CS3" t="n">
-        <v>12.91883333333333</v>
+        <v>0.237</v>
       </c>
       <c r="CT3" t="n">
-        <v>53.943</v>
+        <v>0.266</v>
       </c>
       <c r="CU3" t="n">
-        <v>0.454</v>
-      </c>
-      <c r="CV3" t="n">
+        <v>0.279</v>
+      </c>
+      <c r="CV3" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="CW3" t="n">
         <v>0.237</v>
       </c>
-      <c r="CW3" t="n">
-        <v>0.266</v>
-      </c>
       <c r="CX3" t="n">
-        <v>0.279</v>
-      </c>
-      <c r="CY3" t="inlineStr">
+        <v>3.752</v>
+      </c>
+      <c r="CY3" t="n">
+        <v>8.432</v>
+      </c>
+      <c r="CZ3" t="n">
+        <v>157.554</v>
+      </c>
+      <c r="DA3" t="n">
+        <v>54.786</v>
+      </c>
+      <c r="DB3" t="inlineStr">
         <is>
           <t>NULL</t>
         </is>
       </c>
-      <c r="CZ3" t="n">
-        <v>0.237</v>
-      </c>
-      <c r="DA3" t="n">
-        <v>3.752</v>
-      </c>
-      <c r="DB3" t="n">
-        <v>8.432</v>
-      </c>
       <c r="DC3" t="n">
-        <v>157.554</v>
+        <v>0.961</v>
       </c>
       <c r="DD3" t="n">
-        <v>54.786</v>
-      </c>
-      <c r="DE3" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="DF3" t="n">
-        <v>0.961</v>
+        <v>340.717</v>
       </c>
     </row>
   </sheetData>

</xml_diff>